<commit_message>
use v2.6.58-snapshot of cedar-artifact-library
</commit_message>
<xml_diff>
--- a/src/main/resources/spreadsheet2templatePath.xlsx
+++ b/src/main/resources/spreadsheet2templatePath.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C431EE-F9EC-F040-BC74-C059197151D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEE1853-90C0-B44B-891E-7682F17B2E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="1100" windowWidth="27640" windowHeight="19560" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
+    <workbookView xWindow="-15760" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{297628F6-E04B-2149-A12F-46F8E7030659}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -667,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9FA6C8-3052-4F44-924C-F8A85A6A2B10}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +725,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>